<commit_message>
Fix review findings: Smoothness of resized images
- Change Resampling/Interpolation method to INTER_AREA
</commit_message>
<xml_diff>
--- a/docs/review-protocol.xlsx
+++ b/docs/review-protocol.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
   <si>
     <t>Findings</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Smoothness of resized images is not good</t>
+  </si>
+  <si>
+    <t>Solution: change Sampling/Interpolation method to INTER_AREA</t>
   </si>
 </sst>
 </file>
@@ -527,7 +530,7 @@
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +540,7 @@
     <col min="3" max="3" width="14.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="42.85546875" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="2" customWidth="1"/>
     <col min="7" max="7" width="42.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -597,7 +600,9 @@
       <c r="E3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="F3" s="5">
+        <v>43716</v>
+      </c>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -616,7 +621,9 @@
       <c r="E4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="5">
+        <v>43716</v>
+      </c>
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -635,7 +642,9 @@
       <c r="E5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="5">
+        <v>43716</v>
+      </c>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -654,7 +663,9 @@
       <c r="E6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="F6" s="5">
+        <v>43716</v>
+      </c>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -673,7 +684,9 @@
       <c r="E7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="5">
+        <v>43716</v>
+      </c>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -690,7 +703,9 @@
       <c r="E8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="5">
+        <v>43716</v>
+      </c>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -705,10 +720,14 @@
         <v>25</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="F9" s="5">
+        <v>43716</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
@@ -1537,7 +1556,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C100">
       <formula1>findings_list</formula1>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A100">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A100 F3:F9">
       <formula1>43695</formula1>
       <formula2>43830</formula2>
     </dataValidation>

</xml_diff>